<commit_message>
(1) Load initial data; (2) Modify home page with general information
</commit_message>
<xml_diff>
--- a/Mercury-Database/_support/Tests.xlsx
+++ b/Mercury-Database/_support/Tests.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao.godinho\Documents\MIND_SOURCE\_LAB\Repos\github\jppg\Mercury\Mercury-Database\_support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2CB4D157-C314-4874-AD1A-013E7B1BBC19}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1354C49D-69B7-4151-B7C2-CFBC24D14E85}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{951E8F8E-1D76-4B39-B8E2-1718E7A211EB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{951E8F8E-1D76-4B39-B8E2-1718E7A211EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="CF" sheetId="3" r:id="rId3"/>
+    <sheet name="PP" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
   <si>
     <t>vencimento</t>
   </si>
@@ -90,6 +91,105 @@
   </si>
   <si>
     <t>custo anual actual</t>
+  </si>
+  <si>
+    <t>Rubrica</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Fev</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>Abr</t>
+  </si>
+  <si>
+    <t>Mai</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>Ago</t>
+  </si>
+  <si>
+    <t>Set</t>
+  </si>
+  <si>
+    <t>Out</t>
+  </si>
+  <si>
+    <t>Nov</t>
+  </si>
+  <si>
+    <t>Dez</t>
+  </si>
+  <si>
+    <t>Vencimento</t>
+  </si>
+  <si>
+    <t>IHT</t>
+  </si>
+  <si>
+    <t>Premio</t>
+  </si>
+  <si>
+    <t>Prop Ferias</t>
+  </si>
+  <si>
+    <t>Prop Sub Natal</t>
+  </si>
+  <si>
+    <t>Abonos sujeitos a impostos</t>
+  </si>
+  <si>
+    <t>Sub Refeição</t>
+  </si>
+  <si>
+    <t>Ajudas Custo</t>
+  </si>
+  <si>
+    <t>Abonos Isentos de Imposto</t>
+  </si>
+  <si>
+    <t>Totais de abonos</t>
+  </si>
+  <si>
+    <t>Encargos Sociais</t>
+  </si>
+  <si>
+    <t>Comunicacões</t>
+  </si>
+  <si>
+    <t>Telemovel</t>
+  </si>
+  <si>
+    <t>Seguro Acidentes Trabalho</t>
+  </si>
+  <si>
+    <t>Seg. Higiene, Saude no Trabalho</t>
+  </si>
+  <si>
+    <t>Seg de Saude</t>
+  </si>
+  <si>
+    <t>Custo Ano Actual</t>
+  </si>
+  <si>
+    <t>Rúbrica</t>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -99,7 +199,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,8 +222,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -142,6 +249,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -157,7 +294,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -165,6 +302,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -483,7 +626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC01A939-1811-40D7-850B-853481FC5DC3}">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
@@ -579,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BB6C760-3FA4-4D0C-9428-6CBB12CC4505}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -791,4 +934,1054 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9AE043D-6C1B-4FAE-B9FE-0005BB91AEDC}">
+  <dimension ref="A1:P18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2">
+        <v>1660</v>
+      </c>
+      <c r="D2" s="5">
+        <f>$B$2</f>
+        <v>1660</v>
+      </c>
+      <c r="E2" s="5">
+        <f t="shared" ref="E2:O2" si="0">$B$2</f>
+        <v>1660</v>
+      </c>
+      <c r="F2" s="5">
+        <f t="shared" si="0"/>
+        <v>1660</v>
+      </c>
+      <c r="G2" s="5">
+        <f t="shared" si="0"/>
+        <v>1660</v>
+      </c>
+      <c r="H2" s="5">
+        <f t="shared" si="0"/>
+        <v>1660</v>
+      </c>
+      <c r="I2" s="5">
+        <f t="shared" si="0"/>
+        <v>1660</v>
+      </c>
+      <c r="J2" s="5">
+        <f t="shared" si="0"/>
+        <v>1660</v>
+      </c>
+      <c r="K2" s="5">
+        <f t="shared" si="0"/>
+        <v>1660</v>
+      </c>
+      <c r="L2" s="5">
+        <f t="shared" si="0"/>
+        <v>1660</v>
+      </c>
+      <c r="M2" s="5">
+        <f t="shared" si="0"/>
+        <v>1660</v>
+      </c>
+      <c r="N2" s="5">
+        <f t="shared" si="0"/>
+        <v>1660</v>
+      </c>
+      <c r="O2" s="5">
+        <f t="shared" si="0"/>
+        <v>1660</v>
+      </c>
+      <c r="P2" s="5">
+        <f t="shared" ref="P2:P6" si="1">SUM(D2:O2)</f>
+        <v>19920</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3">
+        <v>332</v>
+      </c>
+      <c r="D3" s="5">
+        <f>$B$3</f>
+        <v>332</v>
+      </c>
+      <c r="E3" s="5">
+        <f t="shared" ref="E3:O3" si="2">$B$3</f>
+        <v>332</v>
+      </c>
+      <c r="F3" s="5">
+        <f t="shared" si="2"/>
+        <v>332</v>
+      </c>
+      <c r="G3" s="5">
+        <f t="shared" si="2"/>
+        <v>332</v>
+      </c>
+      <c r="H3" s="5">
+        <f t="shared" si="2"/>
+        <v>332</v>
+      </c>
+      <c r="I3" s="5">
+        <f t="shared" si="2"/>
+        <v>332</v>
+      </c>
+      <c r="J3" s="5">
+        <f t="shared" si="2"/>
+        <v>332</v>
+      </c>
+      <c r="K3" s="5">
+        <f t="shared" si="2"/>
+        <v>332</v>
+      </c>
+      <c r="L3" s="5">
+        <f t="shared" si="2"/>
+        <v>332</v>
+      </c>
+      <c r="M3" s="5">
+        <f t="shared" si="2"/>
+        <v>332</v>
+      </c>
+      <c r="N3" s="5">
+        <f t="shared" si="2"/>
+        <v>332</v>
+      </c>
+      <c r="O3" s="5">
+        <f t="shared" si="2"/>
+        <v>332</v>
+      </c>
+      <c r="P3" s="5">
+        <f t="shared" si="1"/>
+        <v>3984</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5">
+        <v>166</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5">
+        <f>SUM(K2:K3)</f>
+        <v>1992</v>
+      </c>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5">
+        <f t="shared" si="1"/>
+        <v>1992</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6">
+        <v>138.33000000000001</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5">
+        <f>O2</f>
+        <v>1660</v>
+      </c>
+      <c r="P6" s="5">
+        <f t="shared" si="1"/>
+        <v>1660</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="7">
+        <v>2296.33</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8">
+        <v>160.22999999999999</v>
+      </c>
+      <c r="D8" s="5">
+        <f>$B$8</f>
+        <v>160.22999999999999</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" ref="E8:O8" si="3">$B$8</f>
+        <v>160.22999999999999</v>
+      </c>
+      <c r="F8" s="5">
+        <f t="shared" si="3"/>
+        <v>160.22999999999999</v>
+      </c>
+      <c r="G8" s="5">
+        <f t="shared" si="3"/>
+        <v>160.22999999999999</v>
+      </c>
+      <c r="H8" s="5">
+        <f t="shared" si="3"/>
+        <v>160.22999999999999</v>
+      </c>
+      <c r="I8" s="5">
+        <f t="shared" si="3"/>
+        <v>160.22999999999999</v>
+      </c>
+      <c r="J8" s="5">
+        <f t="shared" si="3"/>
+        <v>160.22999999999999</v>
+      </c>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5">
+        <f t="shared" si="3"/>
+        <v>160.22999999999999</v>
+      </c>
+      <c r="M8" s="5">
+        <f t="shared" si="3"/>
+        <v>160.22999999999999</v>
+      </c>
+      <c r="N8" s="5">
+        <f t="shared" si="3"/>
+        <v>160.22999999999999</v>
+      </c>
+      <c r="O8" s="5">
+        <f t="shared" si="3"/>
+        <v>160.22999999999999</v>
+      </c>
+      <c r="P8" s="5">
+        <f t="shared" ref="P8:P9" si="4">SUM(D8:O8)</f>
+        <v>1762.53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9">
+        <v>250.95</v>
+      </c>
+      <c r="D9" s="5">
+        <f>$B$9</f>
+        <v>250.95</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" ref="E9:O9" si="5">$B$9</f>
+        <v>250.95</v>
+      </c>
+      <c r="F9" s="5">
+        <f t="shared" si="5"/>
+        <v>250.95</v>
+      </c>
+      <c r="G9" s="5">
+        <f t="shared" si="5"/>
+        <v>250.95</v>
+      </c>
+      <c r="H9" s="5">
+        <f t="shared" si="5"/>
+        <v>250.95</v>
+      </c>
+      <c r="I9" s="5">
+        <f t="shared" si="5"/>
+        <v>250.95</v>
+      </c>
+      <c r="J9" s="5">
+        <f t="shared" si="5"/>
+        <v>250.95</v>
+      </c>
+      <c r="K9" s="5">
+        <f t="shared" si="5"/>
+        <v>250.95</v>
+      </c>
+      <c r="L9" s="5">
+        <f t="shared" si="5"/>
+        <v>250.95</v>
+      </c>
+      <c r="M9" s="5">
+        <f t="shared" si="5"/>
+        <v>250.95</v>
+      </c>
+      <c r="N9" s="5">
+        <f t="shared" si="5"/>
+        <v>250.95</v>
+      </c>
+      <c r="O9" s="5">
+        <f t="shared" si="5"/>
+        <v>250.95</v>
+      </c>
+      <c r="P9" s="5">
+        <f t="shared" si="4"/>
+        <v>3011.3999999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="8">
+        <v>411.18</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11">
+        <v>2707.51</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12">
+        <v>545.38</v>
+      </c>
+      <c r="D12" s="5">
+        <f>$B$12</f>
+        <v>545.38</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" ref="E12:O12" si="6">$B$12</f>
+        <v>545.38</v>
+      </c>
+      <c r="F12" s="5">
+        <f t="shared" si="6"/>
+        <v>545.38</v>
+      </c>
+      <c r="G12" s="5">
+        <f t="shared" si="6"/>
+        <v>545.38</v>
+      </c>
+      <c r="H12" s="5">
+        <f t="shared" si="6"/>
+        <v>545.38</v>
+      </c>
+      <c r="I12" s="5">
+        <f t="shared" si="6"/>
+        <v>545.38</v>
+      </c>
+      <c r="J12" s="5">
+        <f t="shared" si="6"/>
+        <v>545.38</v>
+      </c>
+      <c r="K12" s="5">
+        <f t="shared" si="6"/>
+        <v>545.38</v>
+      </c>
+      <c r="L12" s="5">
+        <f t="shared" si="6"/>
+        <v>545.38</v>
+      </c>
+      <c r="M12" s="5">
+        <f t="shared" si="6"/>
+        <v>545.38</v>
+      </c>
+      <c r="N12" s="5">
+        <f t="shared" si="6"/>
+        <v>545.38</v>
+      </c>
+      <c r="O12" s="5">
+        <f t="shared" si="6"/>
+        <v>545.38</v>
+      </c>
+      <c r="P12" s="5">
+        <f t="shared" ref="P12:P17" si="7">SUM(D12:O12)</f>
+        <v>6544.56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13">
+        <v>10.34</v>
+      </c>
+      <c r="D13" s="5">
+        <f>$B13</f>
+        <v>10.34</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" ref="E13:O17" si="8">$B13</f>
+        <v>10.34</v>
+      </c>
+      <c r="F13" s="5">
+        <f t="shared" si="8"/>
+        <v>10.34</v>
+      </c>
+      <c r="G13" s="5">
+        <f t="shared" si="8"/>
+        <v>10.34</v>
+      </c>
+      <c r="H13" s="5">
+        <f t="shared" si="8"/>
+        <v>10.34</v>
+      </c>
+      <c r="I13" s="5">
+        <f t="shared" si="8"/>
+        <v>10.34</v>
+      </c>
+      <c r="J13" s="5">
+        <f t="shared" si="8"/>
+        <v>10.34</v>
+      </c>
+      <c r="K13" s="5">
+        <f t="shared" si="8"/>
+        <v>10.34</v>
+      </c>
+      <c r="L13" s="5">
+        <f t="shared" si="8"/>
+        <v>10.34</v>
+      </c>
+      <c r="M13" s="5">
+        <f t="shared" si="8"/>
+        <v>10.34</v>
+      </c>
+      <c r="N13" s="5">
+        <f t="shared" si="8"/>
+        <v>10.34</v>
+      </c>
+      <c r="O13" s="5">
+        <f t="shared" si="8"/>
+        <v>10.34</v>
+      </c>
+      <c r="P13" s="5">
+        <f t="shared" si="7"/>
+        <v>124.08000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14">
+        <v>0.03</v>
+      </c>
+      <c r="D14" s="5">
+        <f t="shared" ref="D14:D17" si="9">$B14</f>
+        <v>0.03</v>
+      </c>
+      <c r="E14" s="5">
+        <f t="shared" si="8"/>
+        <v>0.03</v>
+      </c>
+      <c r="F14" s="5">
+        <f t="shared" si="8"/>
+        <v>0.03</v>
+      </c>
+      <c r="G14" s="5">
+        <f t="shared" si="8"/>
+        <v>0.03</v>
+      </c>
+      <c r="H14" s="5">
+        <f t="shared" si="8"/>
+        <v>0.03</v>
+      </c>
+      <c r="I14" s="5">
+        <f t="shared" si="8"/>
+        <v>0.03</v>
+      </c>
+      <c r="J14" s="5">
+        <f t="shared" si="8"/>
+        <v>0.03</v>
+      </c>
+      <c r="K14" s="5">
+        <f t="shared" si="8"/>
+        <v>0.03</v>
+      </c>
+      <c r="L14" s="5">
+        <f t="shared" si="8"/>
+        <v>0.03</v>
+      </c>
+      <c r="M14" s="5">
+        <f t="shared" si="8"/>
+        <v>0.03</v>
+      </c>
+      <c r="N14" s="5">
+        <f t="shared" si="8"/>
+        <v>0.03</v>
+      </c>
+      <c r="O14" s="5">
+        <f t="shared" si="8"/>
+        <v>0.03</v>
+      </c>
+      <c r="P14" s="5">
+        <f t="shared" si="7"/>
+        <v>0.3600000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15">
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="D15" s="5">
+        <f t="shared" si="9"/>
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="E15" s="5">
+        <f t="shared" si="8"/>
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="F15" s="5">
+        <f t="shared" si="8"/>
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="G15" s="5">
+        <f t="shared" si="8"/>
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="H15" s="5">
+        <f t="shared" si="8"/>
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="I15" s="5">
+        <f t="shared" si="8"/>
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="J15" s="5">
+        <f t="shared" si="8"/>
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="K15" s="5">
+        <f t="shared" si="8"/>
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="L15" s="5">
+        <f t="shared" si="8"/>
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="M15" s="5">
+        <f t="shared" si="8"/>
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="N15" s="5">
+        <f t="shared" si="8"/>
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="O15" s="5">
+        <f t="shared" si="8"/>
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="P15" s="5">
+        <f t="shared" si="7"/>
+        <v>96.479999999999961</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="D16" s="5">
+        <f t="shared" si="9"/>
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="E16" s="5">
+        <f t="shared" si="8"/>
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="F16" s="5">
+        <f t="shared" si="8"/>
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="G16" s="5">
+        <f t="shared" si="8"/>
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="H16" s="5">
+        <f t="shared" si="8"/>
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="I16" s="5">
+        <f t="shared" si="8"/>
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="J16" s="5">
+        <f t="shared" si="8"/>
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="K16" s="5">
+        <f t="shared" si="8"/>
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="L16" s="5">
+        <f t="shared" si="8"/>
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="M16" s="5">
+        <f t="shared" si="8"/>
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="N16" s="5">
+        <f t="shared" si="8"/>
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="O16" s="5">
+        <f t="shared" si="8"/>
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="P16" s="5">
+        <f t="shared" si="7"/>
+        <v>24.84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17">
+        <v>24.57</v>
+      </c>
+      <c r="D17" s="5">
+        <f t="shared" si="9"/>
+        <v>24.57</v>
+      </c>
+      <c r="E17" s="5">
+        <f t="shared" si="8"/>
+        <v>24.57</v>
+      </c>
+      <c r="F17" s="5">
+        <f t="shared" si="8"/>
+        <v>24.57</v>
+      </c>
+      <c r="G17" s="5">
+        <f t="shared" si="8"/>
+        <v>24.57</v>
+      </c>
+      <c r="H17" s="5">
+        <f t="shared" si="8"/>
+        <v>24.57</v>
+      </c>
+      <c r="I17" s="5">
+        <f t="shared" si="8"/>
+        <v>24.57</v>
+      </c>
+      <c r="J17" s="5">
+        <f t="shared" si="8"/>
+        <v>24.57</v>
+      </c>
+      <c r="K17" s="5">
+        <f t="shared" si="8"/>
+        <v>24.57</v>
+      </c>
+      <c r="L17" s="5">
+        <f t="shared" si="8"/>
+        <v>24.57</v>
+      </c>
+      <c r="M17" s="5">
+        <f t="shared" si="8"/>
+        <v>24.57</v>
+      </c>
+      <c r="N17" s="5">
+        <f t="shared" si="8"/>
+        <v>24.57</v>
+      </c>
+      <c r="O17" s="5">
+        <f t="shared" si="8"/>
+        <v>24.57</v>
+      </c>
+      <c r="P17" s="5">
+        <f t="shared" si="7"/>
+        <v>294.83999999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="11">
+        <v>3297.94</v>
+      </c>
+      <c r="D18" s="5">
+        <f>SUM(D2:D17)</f>
+        <v>2993.6100000000006</v>
+      </c>
+      <c r="E18" s="5">
+        <f t="shared" ref="E18:O18" si="10">SUM(E2:E17)</f>
+        <v>2993.6100000000006</v>
+      </c>
+      <c r="F18" s="5">
+        <f t="shared" si="10"/>
+        <v>2993.6100000000006</v>
+      </c>
+      <c r="G18" s="5">
+        <f t="shared" si="10"/>
+        <v>2993.6100000000006</v>
+      </c>
+      <c r="H18" s="5">
+        <f t="shared" si="10"/>
+        <v>2993.6100000000006</v>
+      </c>
+      <c r="I18" s="5">
+        <f t="shared" si="10"/>
+        <v>2993.6100000000006</v>
+      </c>
+      <c r="J18" s="5">
+        <f t="shared" si="10"/>
+        <v>2993.6100000000006</v>
+      </c>
+      <c r="K18" s="5">
+        <f t="shared" si="10"/>
+        <v>4825.3799999999992</v>
+      </c>
+      <c r="L18" s="5">
+        <f t="shared" si="10"/>
+        <v>2993.6100000000006</v>
+      </c>
+      <c r="M18" s="5">
+        <f t="shared" si="10"/>
+        <v>2993.6100000000006</v>
+      </c>
+      <c r="N18" s="5">
+        <f t="shared" si="10"/>
+        <v>2993.6100000000006</v>
+      </c>
+      <c r="O18" s="5">
+        <f t="shared" si="10"/>
+        <v>4653.6099999999988</v>
+      </c>
+      <c r="P18" s="5">
+        <f>SUM(D18:O18)</f>
+        <v>39415.090000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BF92520-BF9D-4714-BE6D-0E4E897D7C1C}">
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4">
+        <v>46.92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6">
+        <v>108.33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="7">
+        <v>1845.25</v>
+      </c>
+      <c r="C7">
+        <f>SUM(B2:B6)-B4</f>
+        <v>1798.33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8">
+        <v>160.22999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9">
+        <v>197.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="8">
+        <v>357.63</v>
+      </c>
+      <c r="C10">
+        <f>SUM(B8:B9)</f>
+        <v>357.63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11">
+        <v>2202.88</v>
+      </c>
+      <c r="C11">
+        <f>C7+C10</f>
+        <v>2155.96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12">
+        <v>427.1</v>
+      </c>
+      <c r="C12">
+        <f>C7*23.75%</f>
+        <v>427.10337499999997</v>
+      </c>
+      <c r="D12">
+        <f>B12/B7</f>
+        <v>0.23145915187643951</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13">
+        <v>10.34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15">
+        <v>6.46</v>
+      </c>
+      <c r="C15">
+        <f>C7* 0.0035</f>
+        <v>6.2941549999999999</v>
+      </c>
+      <c r="D15">
+        <f>B7*0.0035</f>
+        <v>6.4583750000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16">
+        <v>2.0699999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17">
+        <v>24.57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="10">
+        <v>2673</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>